<commit_message>
Able to get data in list from excel input
</commit_message>
<xml_diff>
--- a/MTH_361_Project_1_Data.xlsx
+++ b/MTH_361_Project_1_Data.xlsx
@@ -2,10 +2,10 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\David\Documents\Statistics_Project_1\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,39 +24,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
-    <t>Home</t>
+    <t>home</t>
   </si>
   <si>
-    <t>Away</t>
-  </si>
-  <si>
-    <t>Bating Average for University of Portland Baseball Team (2016)</t>
-  </si>
-  <si>
-    <t>Ho</t>
-  </si>
-  <si>
-    <t>mu_h = mu_a</t>
-  </si>
-  <si>
-    <t>Ha</t>
-  </si>
-  <si>
-    <t>mu_h &gt; mu_a</t>
-  </si>
-  <si>
-    <t>95% CI</t>
-  </si>
-  <si>
-    <t>alpha = .05</t>
+    <t>away</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -368,332 +347,348 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C62"/>
+  <dimension ref="A1:B42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="A63" sqref="A63"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>2</v>
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>1</v>
+      <c r="A2">
+        <v>112</v>
+      </c>
+      <c r="B2">
+        <v>92</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>90</v>
+      </c>
       <c r="B3">
-        <v>0.32400000000000001</v>
+        <v>106</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>115</v>
+      </c>
       <c r="B4">
-        <v>0.29199999999999998</v>
+        <v>108</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>103</v>
+      </c>
       <c r="B5">
-        <v>0.27600000000000002</v>
+        <v>104</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>101</v>
+      </c>
       <c r="B6">
-        <v>0.26300000000000001</v>
+        <v>100</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>0.26200000000000001</v>
+        <v>102</v>
+      </c>
+      <c r="B7">
+        <v>94</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>0.253</v>
+        <v>88</v>
+      </c>
+      <c r="B8">
+        <v>80</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>0.26400000000000001</v>
+        <v>108</v>
+      </c>
+      <c r="B9">
+        <v>103</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>0.26700000000000002</v>
+        <v>112</v>
+      </c>
+      <c r="B10">
+        <v>107</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>0.26400000000000001</v>
+        <v>123</v>
+      </c>
+      <c r="B11">
+        <v>87</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>0.27200000000000002</v>
+        <v>110</v>
+      </c>
+      <c r="B12">
+        <v>109</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>0.26700000000000002</v>
+        <v>105</v>
+      </c>
+      <c r="B13">
+        <v>88</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>0.253</v>
+        <v>105</v>
+      </c>
+      <c r="B14">
+        <v>100</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>110</v>
+      </c>
       <c r="B15">
-        <v>0.26200000000000001</v>
+        <v>106</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>78</v>
+      </c>
       <c r="B16">
-        <v>0.25900000000000001</v>
+        <v>90</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>98</v>
+      </c>
       <c r="B17">
-        <v>0.26</v>
+        <v>94</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>108</v>
+      </c>
       <c r="B18">
-        <v>0.26800000000000002</v>
+        <v>109</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>115</v>
+      </c>
       <c r="B19">
-        <v>0.26400000000000001</v>
+        <v>97</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>99</v>
+      </c>
       <c r="B20">
-        <v>0.25900000000000001</v>
+        <v>89</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>98</v>
+      </c>
       <c r="B21">
-        <v>0.251</v>
+        <v>98</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>0.25</v>
+        <v>121</v>
+      </c>
+      <c r="B22">
+        <v>96</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>0.25</v>
+        <v>112</v>
+      </c>
+      <c r="B23">
+        <v>112</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>0.24199999999999999</v>
+        <v>109</v>
+      </c>
+      <c r="B24">
+        <v>116</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>0.23799999999999999</v>
+        <v>96</v>
+      </c>
+      <c r="B25">
+        <v>89</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>0.24099999999999999</v>
+        <v>107</v>
+      </c>
+      <c r="B26">
+        <v>108</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>103</v>
+      </c>
       <c r="B27">
-        <v>0.23799999999999999</v>
+        <v>96</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>0.23699999999999999</v>
+        <v>116</v>
+      </c>
+      <c r="B28">
+        <v>112</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29">
-        <v>0.23599999999999999</v>
+        <v>137</v>
+      </c>
+      <c r="B29">
+        <v>103</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30">
-        <v>0.23300000000000001</v>
+        <v>115</v>
+      </c>
+      <c r="B30">
+        <v>111</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>112</v>
+      </c>
       <c r="B31">
-        <v>0.23100000000000001</v>
+        <v>104</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>105</v>
+      </c>
       <c r="B32">
-        <v>0.23</v>
+        <v>93</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>116</v>
+      </c>
       <c r="B33">
-        <v>0.22700000000000001</v>
+        <v>115</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>121</v>
+      </c>
       <c r="B34">
-        <v>0.23100000000000001</v>
+        <v>103</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>109</v>
+      </c>
       <c r="B35">
-        <v>0.22800000000000001</v>
+        <v>112</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36">
-        <v>0.22700000000000001</v>
+        <v>108</v>
+      </c>
+      <c r="B36">
+        <v>94</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37">
-        <v>0.23200000000000001</v>
+        <v>105</v>
+      </c>
+      <c r="B37">
+        <v>110</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38">
-        <v>0.23300000000000001</v>
+        <v>116</v>
+      </c>
+      <c r="B38">
+        <v>117</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>110</v>
+      </c>
       <c r="B39">
-        <v>0.23300000000000001</v>
+        <v>120</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>120</v>
+      </c>
       <c r="B40">
-        <v>0.23400000000000001</v>
+        <v>94</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>105</v>
+      </c>
       <c r="B41">
-        <v>0.23499999999999999</v>
+        <v>111</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>107</v>
+      </c>
       <c r="B42">
-        <v>0.23599999999999999</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43">
-        <v>0.23400000000000001</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44">
-        <v>0.23200000000000001</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45">
-        <v>0.23200000000000001</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A46">
-        <v>0.23300000000000001</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A47">
-        <v>0.23599999999999999</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A48">
-        <v>0.23499999999999999</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49">
-        <v>0.23499999999999999</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B50">
-        <v>0.23499999999999999</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B51">
-        <v>0.23300000000000001</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B52">
-        <v>0.23100000000000001</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B53">
-        <v>0.23</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A54">
-        <v>0.22800000000000001</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A55">
-        <v>0.22700000000000001</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A56">
-        <v>0.22500000000000001</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A57">
-        <f>AVERAGE(A3:A56)</f>
-        <v>0.24268965517241381</v>
-      </c>
-      <c r="B57">
-        <f>AVERAGE(B3:B56)</f>
-        <v>0.24919999999999998</v>
-      </c>
-      <c r="C57">
-        <v>0.22500000000000001</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
-        <v>3</v>
-      </c>
-      <c r="B60" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
-        <v>5</v>
-      </c>
-      <c r="B61" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
-        <v>7</v>
-      </c>
-      <c r="B62" t="s">
-        <v>8</v>
+        <v>115</v>
       </c>
     </row>
   </sheetData>

</xml_diff>